<commit_message>
Added Delete customer elements to Task page Created Delete customer test
</commit_message>
<xml_diff>
--- a/actestdata/actidata.xlsx
+++ b/actestdata/actidata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usha1.thayyil\.ssh\com.acti.automation\actestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F79ECF6-0570-45F1-90B7-D8D27D8C2224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD054F1-DAF1-4587-AA0A-36C06F530850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>admin</t>
   </si>
@@ -348,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -364,6 +364,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>